<commit_message>
Widgets Testcases Updated & Automation Test Script updated and Executed Successfully
</commit_message>
<xml_diff>
--- a/FileInput/Widgets.xlsx
+++ b/FileInput/Widgets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Automation Testing Programs\JQueryWebElementsAutomationTesting\FileInput\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation Testing Programs\JQueryWebElementsAutomationTesting\FileInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEEA0D8-D5A6-4A39-BE20-97BDE5D917EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E1EF17-FE6C-4E8A-A6E4-41DE53FB3890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="845" activeTab="2" xr2:uid="{2F09D2FC-9F8C-4591-A842-B775C0FF178F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="845" activeTab="9" xr2:uid="{2F09D2FC-9F8C-4591-A842-B775C0FF178F}"/>
   </bookViews>
   <sheets>
     <sheet name="TS" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="150">
   <si>
     <t>TSID</t>
   </si>
@@ -416,6 +416,84 @@
   </si>
   <si>
     <t>//*[@id="tags"]</t>
+  </si>
+  <si>
+    <t>//iframe[@src='/resources/demos/dialog/default.html']</t>
+  </si>
+  <si>
+    <t>ui-id-1</t>
+  </si>
+  <si>
+    <t>//span[contains(@class,'ui-icon-closethick')]</t>
+  </si>
+  <si>
+    <t>//iframe[@src='/resources/demos/selectmenu/default.html']</t>
+  </si>
+  <si>
+    <t>speed-button</t>
+  </si>
+  <si>
+    <t>//div[contains(@class,'ui-selectmenu-open')]</t>
+  </si>
+  <si>
+    <t>getItemFromListBox</t>
+  </si>
+  <si>
+    <t>//div[contains(@class,'ui-selectmenu-open')]/ul[@id='speed-menu' and @aria-labelledby='speed-button']</t>
+  </si>
+  <si>
+    <t>Fast</t>
+  </si>
+  <si>
+    <t>Get Item From List Box</t>
+  </si>
+  <si>
+    <t>//iframe[@src='/resources/demos/slider/default.html']</t>
+  </si>
+  <si>
+    <t>//span[contains(@class,'ui-slider-handle')]</t>
+  </si>
+  <si>
+    <t>SlideAction</t>
+  </si>
+  <si>
+    <t>E:\Automation Testing Programs\JQueryWebElementsAutomationTesting\ScreenShots\BeforeSliding.png</t>
+  </si>
+  <si>
+    <t>E:\Automation Testing Programs\JQueryWebElementsAutomationTesting\ScreenShots\AfterSliding.png</t>
+  </si>
+  <si>
+    <t>Download Dialog</t>
+  </si>
+  <si>
+    <t>downloadButton</t>
+  </si>
+  <si>
+    <t>Click Download Dialog</t>
+  </si>
+  <si>
+    <t>Click Start Download Button</t>
+  </si>
+  <si>
+    <t>Wait for Iframe</t>
+  </si>
+  <si>
+    <t>Switch to Iframe</t>
+  </si>
+  <si>
+    <t>//iframe[@src='/resources/demos/progressbar/download.html']</t>
+  </si>
+  <si>
+    <t>wait for Start Download Button</t>
+  </si>
+  <si>
+    <t>wait For Dialog Box</t>
+  </si>
+  <si>
+    <t>//div[@aria-describedby='dialog']</t>
+  </si>
+  <si>
+    <t>E:\Automation Testing Programs\JQueryWebElementsAutomationTesting\ScreenShots\Progressbar.png</t>
   </si>
 </sst>
 </file>
@@ -857,7 +935,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,7 +1046,7 @@
         <v>88</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -990,7 +1068,7 @@
         <v>90</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1001,7 +1079,7 @@
         <v>95</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1012,7 +1090,7 @@
         <v>96</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1057,42 +1135,899 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CEC700A-1E73-4EE2-9CC5-FDCA7B3C243E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="97.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="3">
+        <v>10</v>
+      </c>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F7" s="3">
+        <v>10</v>
+      </c>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F9" s="3">
+        <v>10</v>
+      </c>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F11" s="3">
+        <v>10</v>
+      </c>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="10"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="11"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09984510-75C4-463C-91C9-97FAF989FE50}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" s="3">
+        <v>10</v>
+      </c>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F7" s="3">
+        <v>10</v>
+      </c>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F9" s="3">
+        <v>10</v>
+      </c>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" s="3">
+        <v>10</v>
+      </c>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="11"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D5883E4-7A82-4443-B29F-2F74C9CEF25C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P33" sqref="P33"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="97.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="3">
+        <v>10</v>
+      </c>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="11"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2196,7 +3131,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2731,8 +3666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293B8ADE-E583-45CF-8351-FA32EA04396A}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3022,14 +3957,278 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DEFA030-F4FF-4493-887B-AFE6A70681B9}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="97.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="3">
+        <v>10</v>
+      </c>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="11"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>